<commit_message>
COVID 19 template updated
</commit_message>
<xml_diff>
--- a/COVID-19 Resource Planning Data Input Template.xlsx
+++ b/COVID-19 Resource Planning Data Input Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayushi.Goel\OneDrive - EY\COVID Simulator\covid_model\covid_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya.Chawla\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{D80BD72B-E159-40EB-B5D4-D2840E6F2F2A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{ECC9B1C9-76FA-4C78-8B34-E2453F68AA4B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C965711C-EDBB-4056-B5B6-1C2DDB52BDDA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CBC7EA8E-4C05-4DA6-9475-00AFA9545C39}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>District</t>
   </si>
@@ -142,20 +142,84 @@
     <t xml:space="preserve">The tab "SIR Model Inputs" is to be updated by the user. </t>
   </si>
   <si>
-    <t>Anantapur</t>
-  </si>
-  <si>
     <t>Number of patients currently infected with COVID-19 in the administrative unit</t>
   </si>
   <si>
     <t>Currently_infected_COVID_19_Patients</t>
+  </si>
+  <si>
+    <t>Charkhi Dadri</t>
+  </si>
+  <si>
+    <t>Mahendragarh (Narnaul)</t>
+  </si>
+  <si>
+    <t>Ambala</t>
+  </si>
+  <si>
+    <t>Bhiwani</t>
+  </si>
+  <si>
+    <t>Faridabad</t>
+  </si>
+  <si>
+    <t>Fatehabad</t>
+  </si>
+  <si>
+    <t>Gurugram</t>
+  </si>
+  <si>
+    <t>Jhajjar</t>
+  </si>
+  <si>
+    <t>Jind</t>
+  </si>
+  <si>
+    <t>Kaithal</t>
+  </si>
+  <si>
+    <t>Karnal</t>
+  </si>
+  <si>
+    <t>Kurukshetra</t>
+  </si>
+  <si>
+    <t>Nuh</t>
+  </si>
+  <si>
+    <t>Palwal</t>
+  </si>
+  <si>
+    <t>Panchkula</t>
+  </si>
+  <si>
+    <t>Panipat</t>
+  </si>
+  <si>
+    <t>Rewari</t>
+  </si>
+  <si>
+    <t>Rohtak</t>
+  </si>
+  <si>
+    <t>Sirsa</t>
+  </si>
+  <si>
+    <t>Sonipat</t>
+  </si>
+  <si>
+    <t>Yamunanagar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,12 +250,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -214,8 +272,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,7 +295,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,32 +416,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -386,12 +458,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{F298D2BD-6282-4863-9C85-ED696948B540}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,7 +666,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" w="9525">
+              <a14:hiddenLine xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -6612,8 +6704,8 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6625,67 +6717,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="11"/>
+      <c r="A1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
+      <c r="A2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
+      <c r="A3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
+      <c r="A9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
+      <c r="A10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
+      <c r="A15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="11" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -6696,185 +6788,185 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="17" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="17" t="s">
+      <c r="A18" s="5"/>
+      <c r="B18" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="16">
         <v>360000</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="19" t="s">
+      <c r="A19" s="5"/>
+      <c r="B19" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="16">
         <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="17" t="s">
+      <c r="A20" s="5"/>
+      <c r="B20" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="16">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="17"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="21"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="16"/>
     </row>
     <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="20">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="21">
+      <c r="E27" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="21">
+      <c r="E28" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="17">
         <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="26"/>
+      <c r="A32" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6888,149 +6980,438 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="31" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="4">
-        <v>4083315</v>
-      </c>
-      <c r="C2" s="4">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4">
-        <v>4</v>
-      </c>
-      <c r="E2" s="28">
-        <v>0.03</v>
-      </c>
-      <c r="F2" s="4">
-        <v>14</v>
-      </c>
-      <c r="G2" s="28">
-        <v>0.03</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="L2" s="6">
-        <v>100</v>
-      </c>
+      <c r="A2" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="27"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
+      <c r="A3" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="27"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="27"/>
+      <c r="A4" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="27"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="27"/>
+      <c r="A5" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="27"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="27"/>
+      <c r="A6" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="27"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="27"/>
+      <c r="A7" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="27"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="27"/>
+      <c r="A8" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="27"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="27"/>
+      <c r="A9" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="27"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="27"/>
+      <c r="A10" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="27"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="27"/>
+      <c r="A11" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="27"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="27"/>
+      <c r="A12" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="27"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="27"/>
+      <c r="A13" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="27"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="27"/>
+    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="27"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="27"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="25"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="27"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="27"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="27"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="27"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="27"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="27"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="27"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="27"/>
     </row>
   </sheetData>
+  <protectedRanges>
+    <protectedRange algorithmName="SHA-512" hashValue="EbIWvWWKA+vjN3BZYtoe6Pzjsmxhi7wk3XCOy0E+4DN8Ua9exaLibuT681g6Un+cYx99/+s0H+7HZBFzSRVeLw==" saltValue="TMabuH0GGGYJ7HkLBOsXzw==" spinCount="100000" sqref="A2:A23" name="Range2"/>
+    <protectedRange algorithmName="SHA-512" hashValue="PtuAYvgubdk/bS/CvivCMW9e5IAUAEApTvYlBUSzUoVaKDc6Zkd3pn+vw51u6konziUbGK7UsyVvBDKTJm3bFw==" saltValue="rv9AL38iyL9uteJIea3nsQ==" spinCount="100000" sqref="B2:B23" name="Range1"/>
+  </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F869FB7CDC4CB94298D700C417F43B14" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5ddc1ed8db2cb07ec0345f40e9965cba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b33d107c-a448-497d-b606-00e85b1f002a" xmlns:ns4="78603c86-20b2-473c-8048-4163dd4c73c8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="185c07f72270aa66c93c84fd1258fc1d" ns3:_="" ns4:_="">
     <xsd:import namespace="b33d107c-a448-497d-b606-00e85b1f002a"/>
@@ -7253,15 +7634,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7269,6 +7641,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77744988-55CF-42DB-AA3F-F428D09E4811}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40EBDB4E-4287-4E57-BFC9-B7BCCD9C2EA9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7287,26 +7667,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77744988-55CF-42DB-AA3F-F428D09E4811}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{993809F6-BCE1-4108-A471-1792A410B738}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="78603c86-20b2-473c-8048-4163dd4c73c8"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b33d107c-a448-497d-b606-00e85b1f002a"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b33d107c-a448-497d-b606-00e85b1f002a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>